<commit_message>
new report added omega southshore
</commit_message>
<xml_diff>
--- a/Documents/UiPath/TPL_Vendor_Report_Process/Data/Config.xlsx
+++ b/Documents/UiPath/TPL_Vendor_Report_Process/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prasanth\Documents\UiPath\TPL_Vendor_Report_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C73DBDC-0536-4D27-88D7-5356452E34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DD1F8D-7A9F-40A0-A4D7-A0A0A071140A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -72,18 +72,6 @@
     <t>TPL_GebbsReport_SharePoint_FolderName</t>
   </si>
   <si>
-    <t>TPL_eCW_Productivity_Report_ShareDrive_Path</t>
-  </si>
-  <si>
-    <t>TPL_Gebbs_Report_ShareDrive_Path</t>
-  </si>
-  <si>
-    <t>TPL_eCWProductivity_Report_ShareDrive_Path</t>
-  </si>
-  <si>
-    <t>TPL_omega_NYP_Report_ShareDrive_Path</t>
-  </si>
-  <si>
     <t>TPL_omega_NYP_Report_SharePoint_LibraryName</t>
   </si>
   <si>
@@ -99,12 +87,6 @@
     <t>TPL_omega_UCC_Report_SharePoint_FolderName</t>
   </si>
   <si>
-    <t>TPL_omega_UCC_Report_ShareDrive_Path</t>
-  </si>
-  <si>
-    <t>TPL_GebbsReport_ShareDrive_Path</t>
-  </si>
-  <si>
     <t>TPL_DataBaseName</t>
   </si>
   <si>
@@ -282,16 +264,49 @@
     <t>TPL_OmegaUCCReport_SharePoint_FolderName</t>
   </si>
   <si>
-    <t>TPL_OmegaNYP_Report_ShareDrive_Path</t>
-  </si>
-  <si>
-    <t>TPL_OmegaUCC_Report_ShareDrive_Path</t>
-  </si>
-  <si>
     <t>TPL_eCWproductivityReport_SharePoint_url</t>
   </si>
   <si>
     <t>TPL_Processed_Mail_Folder</t>
+  </si>
+  <si>
+    <t>TPL_Omega_SouthShore_SharePoint_url</t>
+  </si>
+  <si>
+    <t>TPL_Omega_SouthShore_SharePoint_LibraryName</t>
+  </si>
+  <si>
+    <t>TPL_Omega_SouthShore_SharePoint_FolderName</t>
+  </si>
+  <si>
+    <t>TPL_eCWProductivity_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_eCW_Productivity_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_OmegaNYP_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_omega_NYP_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_OmegaUCC_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_omega_UCC_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_GebbsReport_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_Gebbs_Report_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_Omega_SouthShore_ShareDrive_Folder</t>
+  </si>
+  <si>
+    <t>TPL_ShareDrive_URL</t>
   </si>
 </sst>
 </file>
@@ -635,37 +650,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -692,142 +707,142 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -837,10 +852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB0DFBD-CC60-40E0-B91B-E8F4D79C72F7}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +878,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -887,42 +902,42 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -951,90 +966,130 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1071,26 +1126,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>